<commit_message>
rm cancels still in 3rd tab
</commit_message>
<xml_diff>
--- a/excel_reports/Donna_Aaron.xlsx
+++ b/excel_reports/Donna_Aaron.xlsx
@@ -8,59 +8,88 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Last Month NEW" sheetId="2" r:id="rId2"/>
-    <sheet name="Core" sheetId="3" r:id="rId3"/>
+    <sheet name="Core" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Policy Record</t>
   </si>
   <si>
-    <t>Contact Recrod</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
+    <t>Contact Record</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>OA First</t>
+  </si>
+  <si>
+    <t>OA Last</t>
+  </si>
+  <si>
+    <t>Agent First</t>
+  </si>
+  <si>
+    <t>Agent Last</t>
   </si>
   <si>
     <t>Carrier</t>
   </si>
   <si>
-    <t>Commission ID</t>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Plan Type</t>
-  </si>
-  <si>
-    <t>Date Actual Submission</t>
-  </si>
-  <si>
-    <t>Effective Date</t>
-  </si>
-  <si>
-    <t>Date Actual Cancel</t>
-  </si>
-  <si>
-    <t>Date Notified Cancel</t>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>Effective</t>
+  </si>
+  <si>
+    <t>Notified of Cancel</t>
+  </si>
+  <si>
+    <t>Term Date</t>
+  </si>
+  <si>
+    <t>Active?</t>
   </si>
   <si>
     <t>Cancellation Notes</t>
   </si>
   <si>
-    <t>https://app.hubspot.com/contacts/7879306/record/2-8483761/4321868319</t>
-  </si>
-  <si>
-    <t>https://app.hubspot.com/contacts/7879306/contact/25209901</t>
+    <t>Eligible for Residual</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Commissionable?</t>
+  </si>
+  <si>
+    <t>MSP and Residual</t>
+  </si>
+  <si>
+    <t>MAP and Residual</t>
+  </si>
+  <si>
+    <t>4321868319</t>
+  </si>
+  <si>
+    <t>25209901</t>
   </si>
   <si>
     <t>Peggy</t>
@@ -69,99 +98,36 @@
     <t>SCHULBERG</t>
   </si>
   <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>Musick</t>
+  </si>
+  <si>
+    <t>Donna</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
     <t>AARP</t>
   </si>
   <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Supplemental</t>
+  </si>
+  <si>
     <t>110 - Submitted</t>
   </si>
   <si>
-    <t>Supplemental</t>
-  </si>
-  <si>
     <t>12-05-2022</t>
   </si>
   <si>
     <t>01-01-2023</t>
   </si>
   <si>
-    <t>Contact Record</t>
-  </si>
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Last</t>
-  </si>
-  <si>
-    <t>OA First</t>
-  </si>
-  <si>
-    <t>OA Last</t>
-  </si>
-  <si>
-    <t>Agent First</t>
-  </si>
-  <si>
-    <t>Agent Last</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Submitted</t>
-  </si>
-  <si>
-    <t>Effective</t>
-  </si>
-  <si>
-    <t>Notified of Cancel</t>
-  </si>
-  <si>
-    <t>Term Date</t>
-  </si>
-  <si>
-    <t>Active?</t>
-  </si>
-  <si>
-    <t>Eligible for Residual</t>
-  </si>
-  <si>
-    <t>Residual</t>
-  </si>
-  <si>
-    <t>Commissionable?</t>
-  </si>
-  <si>
-    <t>MSP and Residual</t>
-  </si>
-  <si>
-    <t>MAP and Residual</t>
-  </si>
-  <si>
-    <t>4321868319</t>
-  </si>
-  <si>
-    <t>25209901</t>
-  </si>
-  <si>
-    <t>Josh</t>
-  </si>
-  <si>
-    <t>Musick</t>
-  </si>
-  <si>
-    <t>Donna</t>
-  </si>
-  <si>
-    <t>Aaron</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
     <t>False</t>
   </si>
   <si>
@@ -205,9 +171,6 @@
   </si>
   <si>
     <t>Total Core Plan Submissions Last Month</t>
-  </si>
-  <si>
-    <t>Core Plan Cancelations Posted Last Month</t>
   </si>
   <si>
     <t>Residuals</t>
@@ -288,19 +251,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -322,12 +285,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -344,17 +307,14 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -662,35 +622,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B5" s="4">
         <f>B3+B4-B2</f>
@@ -699,7 +659,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2">
         <v>-30</v>
@@ -707,30 +667,30 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B8" s="4">
         <f>SUM(B5:B7)</f>
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B9" s="5">
         <f>MAX(0, B8*150)</f>
@@ -739,41 +699,33 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B17" s="5">
         <f>SUM(Core!T:T)</f>
@@ -782,22 +734,22 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -805,7 +757,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B23">
         <f>-B20+B21+B22</f>
@@ -814,7 +766,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B24" s="5">
         <f>B23*50</f>
@@ -823,17 +775,17 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
@@ -841,7 +793,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B29">
         <f>-B26+B27+B28</f>
@@ -850,7 +802,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B30" s="5">
         <f>B29*100</f>
@@ -864,236 +816,141 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="13" width="25.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="13.7109375" style="8" customWidth="1"/>
-    <col min="3" max="9" width="9.7109375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" style="8" customWidth="1"/>
+    <col min="1" max="2" width="13.7109375" style="6" customWidth="1"/>
+    <col min="3" max="9" width="9.7109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="6" customWidth="1"/>
     <col min="11" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="19" width="10.7109375" style="8" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" style="9" customWidth="1"/>
-    <col min="20" max="20" width="14.7109375" style="8" customWidth="1"/>
+    <col min="17" max="19" width="10.7109375" style="6" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" style="7" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" style="6" customWidth="1"/>
     <col min="21" max="23" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="D2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="E2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="F2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="10" t="s">
+      <c r="G2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="H2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="10" t="s">
+      <c r="I2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="J2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="K2" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="L2" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="M2" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="10" t="s">
+      <c r="N2" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="Q2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="W1" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
-      <c r="A2" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>48</v>
+      <c r="S2" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>